<commit_message>
rewrite synch with if statement #28
</commit_message>
<xml_diff>
--- a/tests/xlsx/selectfromrange_takeif_twice_synced.xlsx
+++ b/tests/xlsx/selectfromrange_takeif_twice_synced.xlsx
@@ -213,10 +213,10 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
+      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="n">
@@ -227,7 +227,7 @@
         <v>#NAME?</v>
       </c>
       <c r="C1" s="1" t="e">
-        <f aca="false">takeif(3,TRUE(),B1,B2)</f>
+        <f aca="false">takeif(3,A1=1,B1,B2)</f>
         <v>#NAME?</v>
       </c>
     </row>
@@ -239,7 +239,7 @@
         <v>6</v>
       </c>
       <c r="C2" s="1" t="e">
-        <f aca="false">takeif(3,TRUE(),A1,B2)</f>
+        <f aca="false">takeif(3,A2=2,A1,B2)</f>
         <v>#NAME?</v>
       </c>
     </row>
@@ -256,10 +256,10 @@
   </conditionalFormatting>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Обычный"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Обычный"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
</xml_diff>